<commit_message>
new file:   Python/.AjusteEstoque/Ajuste.py 	new file:   Python/.Amostra/000 PLANILHA KAZZO ATUAL - SEM SENHA 1.xls 	modified:   Python/.Amostra/Custo.xlsx 	modified:   Python/.Amostra/Planilha.py 	new file:   Python/.Amostra/Planilha2.py 	new file:   Python/.Amostra/Receita.xlsx 	new file:   Python/.Amostra/Teste.py 	new file:   Python/.Amostra/index.py 	new file:   Python/.Amostra/templates/index.html 	modified:   Python/Liberacao/index.py 	modified:   Python/Liberacao/templates/index.html 	deleted:    Python/Pacotes/Consulta SKU.py 	modified:   Python/TOTVS/Fotos.py 	new file:   optionbutton.xlsx
</commit_message>
<xml_diff>
--- a/Python/.Amostra/Custo.xlsx
+++ b/Python/.Amostra/Custo.xlsx
@@ -700,7 +700,7 @@
       <c r="C5" s="2" t="n"/>
       <c r="E5" s="11" t="inlineStr">
         <is>
-          <t>HERING-CALCA MASC. SDP26595 -H1RW</t>
+          <t>HERING CALCA FEM SPA 43395 REF KZ0F</t>
         </is>
       </c>
       <c r="F5" s="2" t="n"/>
@@ -751,11 +751,11 @@
         <v>1</v>
       </c>
       <c r="C7" s="14" t="n">
-        <v>1000047</v>
+        <v>1009196</v>
       </c>
       <c r="E7" s="15" t="inlineStr">
         <is>
-          <t>ETQ  TYVEK 33X50.8</t>
+          <t>ZIPER METAL MED DOURADO YKK</t>
         </is>
       </c>
       <c r="F7" s="16" t="n"/>
@@ -766,7 +766,7 @@
       <c r="K7" s="16" t="n"/>
       <c r="L7" s="16" t="n"/>
       <c r="Q7" s="14" t="n">
-        <v>0.025672</v>
+        <v>0.0033712</v>
       </c>
     </row>
     <row r="8">
@@ -774,12 +774,12 @@
         <v>1</v>
       </c>
       <c r="C8" s="14" t="n">
-        <v>1000062</v>
+        <v>1016752</v>
       </c>
       <c r="D8" s="16" t="n"/>
       <c r="E8" s="15" t="inlineStr">
         <is>
-          <t>ET TAM - K114-(32 AO 62)</t>
+          <t>ET DE MARCA E TAM  ALG 17X85 HRNG</t>
         </is>
       </c>
       <c r="F8" s="16" t="n"/>
@@ -790,20 +790,20 @@
       <c r="K8" s="16" t="n"/>
       <c r="L8" s="16" t="n"/>
       <c r="Q8" s="14" t="n">
-        <v>0.005714400000000001</v>
+        <v>0.06</v>
       </c>
     </row>
     <row r="9">
       <c r="B9" s="14" t="n">
-        <v>1.12</v>
+        <v>1</v>
       </c>
       <c r="C9" s="14" t="n">
-        <v>1001349</v>
+        <v>1016758</v>
       </c>
       <c r="D9" s="16" t="n"/>
       <c r="E9" s="15" t="inlineStr">
         <is>
-          <t>ALGARVE INTENSE 100% ALG 12OZ INDIGO</t>
+          <t>ET DE MOD ALG 15X15 HRNG MASC SKINNY</t>
         </is>
       </c>
       <c r="F9" s="16" t="n"/>
@@ -814,7 +814,7 @@
       <c r="K9" s="16" t="n"/>
       <c r="L9" s="16" t="n"/>
       <c r="Q9" s="14" t="n">
-        <v>7.383040000000001</v>
+        <v>0.031264</v>
       </c>
     </row>
     <row r="10">
@@ -822,12 +822,12 @@
         <v>1</v>
       </c>
       <c r="C10" s="14" t="n">
-        <v>1001554</v>
+        <v>1016824</v>
       </c>
       <c r="D10" s="16" t="n"/>
       <c r="E10" s="15" t="inlineStr">
         <is>
-          <t>BT HERING FLEX RETO 23MM LT DES 0404105</t>
+          <t>BT HERING FLE 1.190.90.L 3</t>
         </is>
       </c>
       <c r="F10" s="16" t="n"/>
@@ -838,20 +838,20 @@
       <c r="K10" s="16" t="n"/>
       <c r="L10" s="16" t="n"/>
       <c r="Q10" s="14" t="n">
-        <v>0.16462</v>
+        <v>0.176</v>
       </c>
     </row>
     <row r="11">
       <c r="B11" s="14" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C11" s="14" t="n">
-        <v>1001816</v>
+        <v>1016826</v>
       </c>
       <c r="D11" s="16" t="n"/>
       <c r="E11" s="15" t="inlineStr">
         <is>
-          <t>ZIP METAL MED NIQUELADO</t>
+          <t>RB HERING 9MM FE.4095.L DES 0570509</t>
         </is>
       </c>
       <c r="F11" s="16" t="n"/>
@@ -862,20 +862,20 @@
       <c r="K11" s="16" t="n"/>
       <c r="L11" s="16" t="n"/>
       <c r="Q11" s="14" t="n">
-        <v>0.3218</v>
+        <v>0.06720000000000001</v>
       </c>
     </row>
     <row r="12">
       <c r="B12" s="14" t="n">
-        <v>0.23</v>
+        <v>1</v>
       </c>
       <c r="C12" s="14" t="n">
-        <v>1004987</v>
+        <v>1016831</v>
       </c>
       <c r="D12" s="16" t="n"/>
       <c r="E12" s="15" t="inlineStr">
         <is>
-          <t>FORRO SOLAR 50%ALG 50%POL LP 1.67</t>
+          <t>ET PU 45X60 HRNG JEANS LAGOM</t>
         </is>
       </c>
       <c r="F12" s="16" t="n"/>
@@ -886,96 +886,94 @@
       <c r="K12" s="16" t="n"/>
       <c r="L12" s="16" t="n"/>
       <c r="Q12" s="14" t="n">
-        <v>0.26956</v>
+        <v>0.176</v>
       </c>
     </row>
     <row r="13">
-      <c r="B13" s="16" t="n"/>
-      <c r="C13" s="16" t="n"/>
+      <c r="B13" s="14" t="n">
+        <v>1.28</v>
+      </c>
+      <c r="C13" s="14" t="n">
+        <v>1017138</v>
+      </c>
       <c r="D13" s="16" t="n"/>
-      <c r="E13" s="16" t="n"/>
-      <c r="F13" s="17" t="n"/>
-      <c r="G13" s="17" t="n"/>
-      <c r="H13" s="17" t="n"/>
-      <c r="I13" s="17" t="n"/>
-      <c r="J13" s="17" t="n"/>
-      <c r="K13" s="17" t="n"/>
+      <c r="E13" s="15" t="inlineStr">
+        <is>
+          <t>IMPORTADO MARTHA 12OZ 99%AL 1%EL LP1,61</t>
+        </is>
+      </c>
+      <c r="F13" s="16" t="n"/>
+      <c r="G13" s="16" t="n"/>
+      <c r="H13" s="16" t="n"/>
+      <c r="I13" s="16" t="n"/>
+      <c r="J13" s="16" t="n"/>
+      <c r="K13" s="16" t="n"/>
       <c r="L13" s="16" t="n"/>
-      <c r="Q13" s="16" t="n"/>
+      <c r="Q13" s="14" t="n">
+        <v>1.5872</v>
+      </c>
     </row>
     <row r="14">
-      <c r="B14" s="16" t="n"/>
-      <c r="C14" s="16" t="n"/>
+      <c r="B14" s="14" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="C14" s="14" t="n">
+        <v>1025750</v>
+      </c>
       <c r="D14" s="16" t="n"/>
-      <c r="E14" s="16" t="n"/>
-      <c r="F14" s="17" t="n"/>
-      <c r="G14" s="17" t="n"/>
-      <c r="H14" s="17" t="n"/>
-      <c r="I14" s="17" t="n"/>
-      <c r="J14" s="17" t="n"/>
-      <c r="K14" s="17" t="n"/>
+      <c r="E14" s="15" t="inlineStr">
+        <is>
+          <t>FORRO CAMPEAO 1,9OZ 67%POL.33%AL LP 1,60</t>
+        </is>
+      </c>
+      <c r="F14" s="16" t="n"/>
+      <c r="G14" s="16" t="n"/>
+      <c r="H14" s="16" t="n"/>
+      <c r="I14" s="16" t="n"/>
+      <c r="J14" s="16" t="n"/>
+      <c r="K14" s="16" t="n"/>
       <c r="L14" s="16" t="n"/>
-      <c r="Q14" s="16" t="n"/>
+      <c r="Q14" s="14" t="n">
+        <v>0.2952</v>
+      </c>
     </row>
     <row r="15">
-      <c r="B15" s="18" t="inlineStr">
-        <is>
-          <t>MANUAIS / LAVAGEM</t>
-        </is>
-      </c>
+      <c r="B15" s="16" t="n"/>
       <c r="C15" s="16" t="n"/>
       <c r="D15" s="16" t="n"/>
       <c r="E15" s="16" t="n"/>
-      <c r="F15" s="16" t="n"/>
-      <c r="G15" s="16" t="n"/>
-      <c r="H15" s="16" t="n"/>
-      <c r="I15" s="16" t="n"/>
-      <c r="J15" s="16" t="n"/>
-      <c r="K15" s="16" t="n"/>
+      <c r="F15" s="17" t="n"/>
+      <c r="G15" s="17" t="n"/>
+      <c r="H15" s="17" t="n"/>
+      <c r="I15" s="17" t="n"/>
+      <c r="J15" s="17" t="n"/>
+      <c r="K15" s="17" t="n"/>
       <c r="L15" s="16" t="n"/>
-      <c r="M15" s="16" t="n"/>
-      <c r="N15" s="16" t="n"/>
-      <c r="O15" s="16" t="n"/>
-      <c r="P15" s="16" t="n"/>
       <c r="Q15" s="16" t="n"/>
     </row>
     <row r="16">
       <c r="B16" s="16" t="n"/>
-      <c r="C16" s="15" t="n">
-        <v>22</v>
-      </c>
+      <c r="C16" s="16" t="n"/>
       <c r="D16" s="16" t="n"/>
-      <c r="E16" s="15" t="inlineStr">
-        <is>
-          <t>COSTURA R$ 6,20</t>
-        </is>
-      </c>
-      <c r="F16" s="16" t="n"/>
-      <c r="G16" s="16" t="n"/>
-      <c r="H16" s="16" t="n"/>
-      <c r="I16" s="16" t="n"/>
-      <c r="J16" s="16" t="n"/>
-      <c r="K16" s="16" t="n"/>
+      <c r="E16" s="16" t="n"/>
+      <c r="F16" s="17" t="n"/>
+      <c r="G16" s="17" t="n"/>
+      <c r="H16" s="17" t="n"/>
+      <c r="I16" s="17" t="n"/>
+      <c r="J16" s="17" t="n"/>
+      <c r="K16" s="17" t="n"/>
       <c r="L16" s="16" t="n"/>
-      <c r="M16" s="16" t="n"/>
-      <c r="N16" s="16" t="n"/>
-      <c r="O16" s="16" t="n"/>
-      <c r="P16" s="16" t="n"/>
-      <c r="Q16" s="15" t="n">
-        <v>6.2</v>
-      </c>
+      <c r="Q16" s="16" t="n"/>
     </row>
     <row r="17">
-      <c r="B17" s="16" t="n"/>
-      <c r="C17" s="15" t="n">
-        <v>82</v>
-      </c>
+      <c r="B17" s="18" t="inlineStr">
+        <is>
+          <t>MANUAIS / LAVAGEM</t>
+        </is>
+      </c>
+      <c r="C17" s="16" t="n"/>
       <c r="D17" s="16" t="n"/>
-      <c r="E17" s="15" t="inlineStr">
-        <is>
-          <t>ACABAMENTO R$ 2,60 NAO USAR</t>
-        </is>
-      </c>
+      <c r="E17" s="16" t="n"/>
       <c r="F17" s="16" t="n"/>
       <c r="G17" s="16" t="n"/>
       <c r="H17" s="16" t="n"/>
@@ -987,37 +985,7 @@
       <c r="N17" s="16" t="n"/>
       <c r="O17" s="16" t="n"/>
       <c r="P17" s="16" t="n"/>
-      <c r="Q17" s="15" t="n">
-        <v>2.6</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="B18" s="16" t="n"/>
-      <c r="C18" s="16" t="n"/>
-      <c r="D18" s="16" t="n"/>
-      <c r="E18" s="16" t="n"/>
-      <c r="F18" s="17" t="n"/>
-      <c r="G18" s="17" t="n"/>
-      <c r="H18" s="17" t="n"/>
-      <c r="I18" s="17" t="n"/>
-      <c r="J18" s="17" t="n"/>
-      <c r="K18" s="17" t="n"/>
-      <c r="L18" s="16" t="n"/>
-      <c r="Q18" s="16" t="n"/>
-    </row>
-    <row r="19">
-      <c r="B19" s="16" t="n"/>
-      <c r="C19" s="16" t="n"/>
-      <c r="D19" s="16" t="n"/>
-      <c r="E19" s="16" t="n"/>
-      <c r="F19" s="17" t="n"/>
-      <c r="G19" s="17" t="n"/>
-      <c r="H19" s="17" t="n"/>
-      <c r="I19" s="17" t="n"/>
-      <c r="J19" s="17" t="n"/>
-      <c r="K19" s="17" t="n"/>
-      <c r="L19" s="16" t="n"/>
-      <c r="Q19" s="16" t="n"/>
+      <c r="Q17" s="16" t="n"/>
     </row>
     <row r="20" ht="5" customHeight="1">
       <c r="B20" s="16" t="n"/>
@@ -1040,7 +1008,7 @@
     <row r="21" ht="24" customHeight="1">
       <c r="B21" s="19" t="inlineStr">
         <is>
-          <t>13/11/2024</t>
+          <t>18/11/2024</t>
         </is>
       </c>
       <c r="C21" s="16" t="n"/>
@@ -1063,7 +1031,7 @@
       <c r="P21" s="16" t="n"/>
       <c r="Q21" s="20" t="inlineStr">
         <is>
-          <t>R$ 9,8045</t>
+          <t>R$ 2,8755</t>
         </is>
       </c>
     </row>
@@ -1093,7 +1061,7 @@
       <c r="P22" s="16" t="n"/>
       <c r="Q22" s="20" t="inlineStr">
         <is>
-          <t>R$ 8,8</t>
+          <t>R$ 0</t>
         </is>
       </c>
     </row>
@@ -1123,7 +1091,7 @@
       <c r="P23" s="16" t="n"/>
       <c r="Q23" s="20" t="inlineStr">
         <is>
-          <t>R$ 18,6045</t>
+          <t>R$ 2,8755</t>
         </is>
       </c>
     </row>
@@ -1231,7 +1199,7 @@
       <c r="P27" s="2" t="n"/>
       <c r="Q27" s="28" t="inlineStr">
         <is>
-          <t>R$ 22,5654</t>
+          <t>R$ 3,6906</t>
         </is>
       </c>
     </row>
@@ -1257,14 +1225,13 @@
       <c r="P28" s="2" t="n"/>
       <c r="Q28" s="28" t="inlineStr">
         <is>
-          <t>R$ 18,8045</t>
+          <t>R$ 3,0755</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="35">
+  <mergeCells count="32">
     <mergeCell ref="E12:L12"/>
-    <mergeCell ref="E18:L18"/>
     <mergeCell ref="E21:L21"/>
     <mergeCell ref="E24:L24"/>
     <mergeCell ref="B22:C22"/>
@@ -1272,16 +1239,15 @@
     <mergeCell ref="E5:L5"/>
     <mergeCell ref="E23:L23"/>
     <mergeCell ref="E8:L8"/>
-    <mergeCell ref="E17:L17"/>
     <mergeCell ref="B21:C21"/>
-    <mergeCell ref="E20:L20"/>
     <mergeCell ref="C3:L3"/>
     <mergeCell ref="B23:C23"/>
     <mergeCell ref="E10:L10"/>
     <mergeCell ref="E28:L28"/>
     <mergeCell ref="E13:L13"/>
-    <mergeCell ref="E19:L19"/>
+    <mergeCell ref="B17:L17"/>
     <mergeCell ref="E9:L9"/>
+    <mergeCell ref="E15:L15"/>
     <mergeCell ref="C4:L4"/>
     <mergeCell ref="E6:L6"/>
     <mergeCell ref="Q3:Q5"/>
@@ -1291,10 +1257,9 @@
     <mergeCell ref="E26:L26"/>
     <mergeCell ref="E7:L7"/>
     <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B15:L15"/>
+    <mergeCell ref="E25:L25"/>
     <mergeCell ref="B1:Q1"/>
     <mergeCell ref="E16:L16"/>
-    <mergeCell ref="E25:L25"/>
     <mergeCell ref="E22:L22"/>
     <mergeCell ref="C2:L2"/>
     <mergeCell ref="B24:C28"/>

</xml_diff>